<commit_message>
fixed timeout bug, improved reward function and, implemented door and key solutions
</commit_message>
<xml_diff>
--- a/src/server/probabilities/1.xlsx
+++ b/src/server/probabilities/1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Parisa\Desktop\AI-Phase2-fall2022\AI_GAME_2022\src\server\probabilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Parisa\PycharmProjects\pythonProject1\src\server\probabilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E84161CD-6EFC-4AFB-8BFA-A7C204E3A1E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3483EE66-622E-4B4B-BF46-5BF49AFA8AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -380,8 +380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.21875" defaultRowHeight="24.45" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -509,13 +509,13 @@
         <v>0</v>
       </c>
       <c r="G4" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H4" s="1">
         <v>0</v>
       </c>
       <c r="I4" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="J4" s="1">
         <v>0</v>
@@ -541,16 +541,16 @@
         <v>0.8</v>
       </c>
       <c r="F5" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
         <v>0.1</v>
       </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
       <c r="I5" s="1">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="J5" s="1">
         <v>0</v>

</xml_diff>